<commit_message>
Format changes inside excel file referred to continents
</commit_message>
<xml_diff>
--- a/toolbox/utilities/privateFS/continents-according-to-our-world-in-data.xlsx
+++ b/toolbox/utilities/privateFS/continents-according-to-our-world-in-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA\toolbox\utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA\toolbox\utilities\privateFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CEBF4B-1F6B-4A8B-AEBF-C0A06CF609B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910A725A-3EAB-4713-BA19-4B5749AC25F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{0F1F91C3-AB88-4B1C-B272-861E8199DE24}"/>
   </bookViews>
@@ -4080,7 +4080,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4236,12 +4236,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -4998,7 +4992,7 @@
   <dimension ref="A1:E286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5009,20 +5003,20 @@
     <col min="4" max="5" width="8.83984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="28.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>1121</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>1122</v>
       </c>
     </row>
@@ -10451,7 +10445,7 @@
   <dimension ref="A1:F263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10463,7 +10457,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>584</v>
       </c>
       <c r="B1" s="1" t="s">

</xml_diff>

<commit_message>
Updated excel file with continents and countries
</commit_message>
<xml_diff>
--- a/toolbox/utilities/privateFS/continents-according-to-our-world-in-data.xlsx
+++ b/toolbox/utilities/privateFS/continents-according-to-our-world-in-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA\toolbox\utilities\privateFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910A725A-3EAB-4713-BA19-4B5749AC25F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805C9D7C-7C3B-44E8-BD61-8922EB326E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{0F1F91C3-AB88-4B1C-B272-861E8199DE24}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{0F1F91C3-AB88-4B1C-B272-861E8199DE24}"/>
   </bookViews>
   <sheets>
     <sheet name="CountryContinent" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="1333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="1332">
   <si>
     <t>Entity</t>
   </si>
@@ -4032,9 +4032,6 @@
   </si>
   <si>
     <t>Turks and Caicos</t>
-  </si>
-  <si>
-    <t>Turks and Caicos Islands;</t>
   </si>
   <si>
     <t>Crimea</t>
@@ -4238,7 +4235,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4424,6 +4421,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -4585,7 +4588,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4600,6 +4603,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4991,8 +4995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801C42A8-5B9E-4875-A425-B285D25643D0}">
   <dimension ref="A1:E286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="A252" sqref="A252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6104,7 +6108,7 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" t="s">
+      <c r="A59" s="6" t="s">
         <v>123</v>
       </c>
       <c r="B59" t="s">
@@ -6294,7 +6298,7 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" t="s">
+      <c r="A69" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B69" t="s">
@@ -10444,8 +10448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334A564C-7700-4F5C-866F-3E76645DC30B}">
   <dimension ref="A1:F263"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15726,8 +15730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17363E50-6B9F-4AD4-8E80-4D0DCC74AF60}">
   <dimension ref="A1:B225"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="B210" sqref="B210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16765,7 +16769,7 @@
         <v>1247</v>
       </c>
       <c r="B129" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -16781,7 +16785,7 @@
         <v>1249</v>
       </c>
       <c r="B131" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -17413,12 +17417,12 @@
         <v>1318</v>
       </c>
       <c r="B210" t="s">
-        <v>1319</v>
+        <v>521</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="B211" t="s">
         <v>533</v>
@@ -17426,7 +17430,7 @@
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="B212" t="s">
         <v>537</v>
@@ -17434,7 +17438,7 @@
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="B213" t="s">
         <v>537</v>
@@ -17442,7 +17446,7 @@
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B214" t="s">
         <v>537</v>
@@ -17450,7 +17454,7 @@
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="B215" t="s">
         <v>537</v>
@@ -17466,7 +17470,7 @@
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B217" t="s">
         <v>539</v>
@@ -17474,7 +17478,7 @@
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B218" t="s">
         <v>539</v>
@@ -17482,7 +17486,7 @@
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="B219" t="s">
         <v>539</v>
@@ -17490,7 +17494,7 @@
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B220" t="s">
         <v>539</v>
@@ -17506,7 +17510,7 @@
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="B222" t="s">
         <v>543</v>
@@ -17514,7 +17518,7 @@
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="B223" t="s">
         <v>543</v>
@@ -17522,7 +17526,7 @@
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="B224" t="s">
         <v>545</v>
@@ -17530,7 +17534,7 @@
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B225" t="s">
         <v>573</v>

</xml_diff>